<commit_message>
working on dataset preparation.
</commit_message>
<xml_diff>
--- a/Evaluations/FoCus-results.xlsx
+++ b/Evaluations/FoCus-results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,7 +515,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.83 ± 0.09</t>
+          <t>0.85 ± 0.09</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -552,32 +552,69 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.64 ± 0.18</t>
+          <t>0.6 ± 0.17</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.73 ± 0.44</t>
+          <t>0.8 ± 0.39</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-0.07 ± 0.7</t>
+          <t>0.03 ± 0.69</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.3 ± 0.64</t>
+          <t>0.34 ± 0.67</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.37 ± 0.23</t>
+          <t>0.4 ± 0.22</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.203 ± 0.00</t>
+          <t>0.149 ± 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Qwen2-5B-DPO</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0.86 ± 0.09</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.39 ± 0.48</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>-0.47 ± 0.76</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.16 ± 0.48</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.22 ± 0.28</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.595 ± 0.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
working on the dataset preprocessing.
</commit_message>
<xml_diff>
--- a/Evaluations/FoCus-results.xlsx
+++ b/Evaluations/FoCus-results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,6 +618,43 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Qwen2-5B-FoCus-length_prior</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.83 ± 0.12</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.48 ± 0.47</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-0.18 ± 0.62</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.32 ± 0.68</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.27 ± 0.19</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.241 ± 0.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
1855 record trainning results are ready
</commit_message>
<xml_diff>
--- a/Evaluations/FoCus-results.xlsx
+++ b/Evaluations/FoCus-results.xlsx
@@ -14,9 +14,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="1">
-  <si>
-    <t/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>response_time</t>
+  </si>
+  <si>
+    <t>Coh-UniEval</t>
+  </si>
+  <si>
+    <t>C Score</t>
+  </si>
+  <si>
+    <t>UE Score</t>
+  </si>
+  <si>
+    <t>Persona Distance</t>
+  </si>
+  <si>
+    <t>Failure Ratio</t>
+  </si>
+  <si>
+    <t>Qwen2-7B-benchmark</t>
+  </si>
+  <si>
+    <t>4.02 ± 0.48</t>
+  </si>
+  <si>
+    <t>0.37 ± 0.48</t>
+  </si>
+  <si>
+    <t>-0.37 ± 0.87</t>
+  </si>
+  <si>
+    <t>0.16 ± 0.48</t>
+  </si>
+  <si>
+    <t>0.22 ± 0.29</t>
+  </si>
+  <si>
+    <t>0.627 ± 0.00</t>
+  </si>
+  <si>
+    <t>Qwen2-5B-avg-1855-complete</t>
+  </si>
+  <si>
+    <t>0.63 ± 0.25</t>
+  </si>
+  <si>
+    <t>0.24 ± 0.42</t>
+  </si>
+  <si>
+    <t>-0.61 ± 0.67</t>
+  </si>
+  <si>
+    <t>0.08 ± 0.35</t>
+  </si>
+  <si>
+    <t>0.16 ± 0.26</t>
+  </si>
+  <si>
+    <t>0.712 ± 0.00</t>
+  </si>
+  <si>
+    <t>Qwen2-5B-length_prior-1855-complete</t>
+  </si>
+  <si>
+    <t>0.45 ± 0.23</t>
+  </si>
+  <si>
+    <t>0.38 ± 0.48</t>
+  </si>
+  <si>
+    <t>-0.53 ± 0.67</t>
+  </si>
+  <si>
+    <t>0.09 ± 0.36</t>
+  </si>
+  <si>
+    <t>0.21 ± 0.27</t>
+  </si>
+  <si>
+    <t>0.608 ± 0.00</t>
   </si>
 </sst>
 </file>
@@ -76,10 +157,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -387,180 +468,111 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="41.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="37.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
-      <c r="A5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
-      <c r="A7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving the current results.
</commit_message>
<xml_diff>
--- a/Evaluations/FoCus-results.xlsx
+++ b/Evaluations/FoCus-results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -655,6 +655,154 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Qwen2-5B-Instruct-simple 12452</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0.2 ± 0.04</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.98 ± 0.08</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.06 ± 0.49</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.21 ± 0.58</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.4 ± 0.13</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.003 ± 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Qwen2-5B-Instruct-perso old</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0.46 ± 0.29</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.92 ± 0.18</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-0.01 ± 0.46</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.27 ± 0.65</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0.31 ± 0.12</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.0 ± 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Qwen2-5B-Instruct-perso check-2304</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0.51 ± 0.25</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.71 ± 0.44</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>-0.13 ± 0.62</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.17 ± 0.52</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0.32 ± 0.2</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.221 ± 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Qwen2-5B-Instruct-perso</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0.89 ± 0.04</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.7 ± 0.45</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.18 ± 0.87</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0.3 ± 0.62</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.44 ± 0.3</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.29 ± 0.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>